<commit_message>
Breathing system + Footsteps on every levels + Peristant audio
+ Script Player_MentalState to adapt player awarness of itself
+ Audio Scripts on every levels
+ System to filter persistant (music...) to non persistant (footsteps...) between leves
~ Footsteps speed
</commit_message>
<xml_diff>
--- a/BehindClosedDoors_SoundAssetList.xlsx
+++ b/BehindClosedDoors_SoundAssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\ISE 2\BehindClosedDoors_Git\BehindClosedDoors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F38AF-7F70-41D3-9E18-4799CA63794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6D877-9A83-4B0D-A529-4BD47BED6044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16080" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="164">
   <si>
     <t>Bible Asset List Library</t>
   </si>
@@ -584,9 +584,6 @@
     <t>RTPC_PLYR_WetFeet</t>
   </si>
   <si>
-    <t>RTPC_PLYR_FS</t>
-  </si>
-  <si>
     <t>Adapt wet level after walking over wet/water surface</t>
   </si>
   <si>
@@ -624,13 +621,20 @@
   </si>
   <si>
     <t>PLYR_FS_Carpet_Sneak</t>
+  </si>
+  <si>
+    <t>Increase over progression (After each Clue) + climax on Tunnel
+Impact on Amb + RTPC_PLYR_SelfConscious minimum &amp; Recovery time</t>
+  </si>
+  <si>
+    <t>RTPC_PLYR_FS_State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +660,13 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -980,6 +991,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1311,8 +1323,8 @@
   </sheetPr>
   <dimension ref="A1:R173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,12 +1352,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1359,14 +1371,14 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="33"/>
+      <c r="Q1" s="34"/>
       <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1400,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1520,7 +1532,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1620,7 +1632,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1959,7 +1971,7 @@
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
         <v>66</v>
@@ -2850,7 +2862,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
@@ -2858,7 +2870,7 @@
       <c r="Q66" s="7"/>
       <c r="R66" s="11"/>
     </row>
-    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="11" t="s">
         <v>106</v>
@@ -2876,7 +2888,7 @@
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
       <c r="M67" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -2884,7 +2896,7 @@
       <c r="Q67" s="7"/>
       <c r="R67" s="11"/>
     </row>
-    <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="7" t="s">
         <v>107</v>
@@ -2902,7 +2914,7 @@
       <c r="K68" s="7"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -2910,7 +2922,7 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="11"/>
     </row>
-    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2924,7 +2936,7 @@
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -2932,7 +2944,7 @@
       <c r="Q69" s="7"/>
       <c r="R69" s="11"/>
     </row>
-    <row r="70" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2946,7 +2958,7 @@
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
@@ -2954,7 +2966,7 @@
       <c r="Q70" s="7"/>
       <c r="R70" s="11"/>
     </row>
-    <row r="71" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>114</v>
       </c>
@@ -2974,7 +2986,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
@@ -2982,7 +2994,7 @@
       <c r="Q71" s="7"/>
       <c r="R71" s="11"/>
     </row>
-    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
         <v>112</v>
@@ -3000,7 +3012,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
@@ -3008,7 +3020,7 @@
       <c r="Q72" s="7"/>
       <c r="R72" s="11"/>
     </row>
-    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="7" t="s">
         <v>113</v>
@@ -3026,7 +3038,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3034,7 +3046,7 @@
       <c r="Q73" s="7"/>
       <c r="R73" s="11"/>
     </row>
-    <row r="74" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="7" t="s">
         <v>118</v>
@@ -3052,7 +3064,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3060,7 +3072,7 @@
       <c r="Q74" s="7"/>
       <c r="R74" s="11"/>
     </row>
-    <row r="75" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
         <v>119</v>
@@ -3078,7 +3090,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
@@ -3104,7 +3116,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3112,7 +3124,7 @@
       <c r="Q76" s="7"/>
       <c r="R76" s="11"/>
     </row>
-    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="7" t="s">
         <v>124</v>
@@ -3130,7 +3142,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
@@ -3138,7 +3150,7 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="11"/>
     </row>
-    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="7" t="s">
         <v>126</v>
@@ -3156,7 +3168,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
@@ -3164,14 +3176,14 @@
       <c r="Q78" s="7"/>
       <c r="R78" s="11"/>
     </row>
-    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="7"/>
@@ -3182,7 +3194,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -3190,7 +3202,7 @@
       <c r="Q79" s="7"/>
       <c r="R79" s="11"/>
     </row>
-    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="30" t="s">
         <v>128</v>
@@ -3208,7 +3220,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
@@ -3216,7 +3228,7 @@
       <c r="Q80" s="7"/>
       <c r="R80" s="11"/>
     </row>
-    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="7" t="s">
         <v>130</v>
@@ -3234,7 +3246,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
@@ -3284,7 +3296,7 @@
       <c r="Q83" s="7"/>
       <c r="R83" s="11"/>
     </row>
-    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>133</v>
       </c>
@@ -3306,7 +3318,7 @@
       <c r="K84" s="7"/>
       <c r="L84" s="7"/>
       <c r="M84" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -3404,7 +3416,7 @@
       <c r="Q88" s="7"/>
       <c r="R88" s="11"/>
     </row>
-    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="7" t="s">
         <v>145</v>
@@ -3622,7 +3634,7 @@
       <c r="Q98" s="7"/>
       <c r="R98" s="11"/>
     </row>
-    <row r="99" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="7" t="s">
         <v>96</v>
@@ -3903,11 +3915,11 @@
     <row r="111" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -4591,12 +4603,12 @@
       <c r="D144" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E144" s="31" t="s">
+      <c r="E144" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F144" s="32"/>
-      <c r="G144" s="32"/>
-      <c r="H144" s="33"/>
+      <c r="F144" s="33"/>
+      <c r="G144" s="33"/>
+      <c r="H144" s="34"/>
       <c r="I144" s="2" t="s">
         <v>5</v>
       </c>
@@ -4708,12 +4720,12 @@
       <c r="D153" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E153" s="31" t="s">
+      <c r="E153" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F153" s="32"/>
-      <c r="G153" s="32"/>
-      <c r="H153" s="33"/>
+      <c r="F153" s="33"/>
+      <c r="G153" s="33"/>
+      <c r="H153" s="34"/>
       <c r="I153" s="2" t="s">
         <v>5</v>
       </c>
@@ -4766,7 +4778,7 @@
     </row>
     <row r="157" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="B157" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>75</v>
@@ -4778,22 +4790,26 @@
         <v>148</v>
       </c>
       <c r="D158" t="s">
+        <v>149</v>
+      </c>
+      <c r="L158" s="27"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B159" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C159" s="31"/>
+      <c r="D159" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="L158" s="27"/>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>149</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="L159" s="27"/>
+    </row>
+    <row r="160" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
         <v>151</v>
       </c>
-      <c r="L159" s="27"/>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>152</v>
+      <c r="D160" s="24" t="s">
+        <v>162</v>
       </c>
       <c r="L160" s="27"/>
     </row>

</xml_diff>

<commit_message>
Revert "Breathing system + Footsteps on every levels + Peristant audio"
This reverts commit 530bc6b4f0910e1a1597afe3ada36a77d115afef.
</commit_message>
<xml_diff>
--- a/BehindClosedDoors_SoundAssetList.xlsx
+++ b/BehindClosedDoors_SoundAssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\ISE 2\BehindClosedDoors_Git\BehindClosedDoors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6D877-9A83-4B0D-A529-4BD47BED6044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F38AF-7F70-41D3-9E18-4799CA63794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16080" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="163">
   <si>
     <t>Bible Asset List Library</t>
   </si>
@@ -584,6 +584,9 @@
     <t>RTPC_PLYR_WetFeet</t>
   </si>
   <si>
+    <t>RTPC_PLYR_FS</t>
+  </si>
+  <si>
     <t>Adapt wet level after walking over wet/water surface</t>
   </si>
   <si>
@@ -621,20 +624,13 @@
   </si>
   <si>
     <t>PLYR_FS_Carpet_Sneak</t>
-  </si>
-  <si>
-    <t>Increase over progression (After each Clue) + climax on Tunnel
-Impact on Amb + RTPC_PLYR_SelfConscious minimum &amp; Recovery time</t>
-  </si>
-  <si>
-    <t>RTPC_PLYR_FS_State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,13 +656,6 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -901,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -991,7 +980,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1323,8 +1311,8 @@
   </sheetPr>
   <dimension ref="A1:R173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,12 +1340,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1371,14 +1359,14 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="34"/>
+      <c r="Q1" s="33"/>
       <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1412,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1532,7 +1520,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1632,7 +1620,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1971,7 +1959,7 @@
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
         <v>66</v>
@@ -2862,7 +2850,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
@@ -2870,7 +2858,7 @@
       <c r="Q66" s="7"/>
       <c r="R66" s="11"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="11" t="s">
         <v>106</v>
@@ -2888,7 +2876,7 @@
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
       <c r="M67" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -2896,7 +2884,7 @@
       <c r="Q67" s="7"/>
       <c r="R67" s="11"/>
     </row>
-    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="7" t="s">
         <v>107</v>
@@ -2914,7 +2902,7 @@
       <c r="K68" s="7"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -2922,7 +2910,7 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="11"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2936,7 +2924,7 @@
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -2944,7 +2932,7 @@
       <c r="Q69" s="7"/>
       <c r="R69" s="11"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2958,7 +2946,7 @@
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
@@ -2966,7 +2954,7 @@
       <c r="Q70" s="7"/>
       <c r="R70" s="11"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>114</v>
       </c>
@@ -2986,7 +2974,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
@@ -2994,7 +2982,7 @@
       <c r="Q71" s="7"/>
       <c r="R71" s="11"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
         <v>112</v>
@@ -3012,7 +3000,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
@@ -3020,7 +3008,7 @@
       <c r="Q72" s="7"/>
       <c r="R72" s="11"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="7" t="s">
         <v>113</v>
@@ -3038,7 +3026,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3046,7 +3034,7 @@
       <c r="Q73" s="7"/>
       <c r="R73" s="11"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="7" t="s">
         <v>118</v>
@@ -3064,7 +3052,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3072,7 +3060,7 @@
       <c r="Q74" s="7"/>
       <c r="R74" s="11"/>
     </row>
-    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
         <v>119</v>
@@ -3090,7 +3078,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
@@ -3116,7 +3104,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3124,7 +3112,7 @@
       <c r="Q76" s="7"/>
       <c r="R76" s="11"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="7" t="s">
         <v>124</v>
@@ -3142,7 +3130,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
@@ -3150,7 +3138,7 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="11"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="7" t="s">
         <v>126</v>
@@ -3168,7 +3156,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
@@ -3176,14 +3164,14 @@
       <c r="Q78" s="7"/>
       <c r="R78" s="11"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="7"/>
@@ -3194,7 +3182,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -3202,7 +3190,7 @@
       <c r="Q79" s="7"/>
       <c r="R79" s="11"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="30" t="s">
         <v>128</v>
@@ -3220,7 +3208,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
@@ -3228,7 +3216,7 @@
       <c r="Q80" s="7"/>
       <c r="R80" s="11"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="7" t="s">
         <v>130</v>
@@ -3246,7 +3234,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
@@ -3296,7 +3284,7 @@
       <c r="Q83" s="7"/>
       <c r="R83" s="11"/>
     </row>
-    <row r="84" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>133</v>
       </c>
@@ -3318,7 +3306,7 @@
       <c r="K84" s="7"/>
       <c r="L84" s="7"/>
       <c r="M84" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -3416,7 +3404,7 @@
       <c r="Q88" s="7"/>
       <c r="R88" s="11"/>
     </row>
-    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="7" t="s">
         <v>145</v>
@@ -3634,7 +3622,7 @@
       <c r="Q98" s="7"/>
       <c r="R98" s="11"/>
     </row>
-    <row r="99" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="7" t="s">
         <v>96</v>
@@ -3915,11 +3903,11 @@
     <row r="111" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -4603,12 +4591,12 @@
       <c r="D144" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E144" s="32" t="s">
+      <c r="E144" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F144" s="33"/>
-      <c r="G144" s="33"/>
-      <c r="H144" s="34"/>
+      <c r="F144" s="32"/>
+      <c r="G144" s="32"/>
+      <c r="H144" s="33"/>
       <c r="I144" s="2" t="s">
         <v>5</v>
       </c>
@@ -4720,12 +4708,12 @@
       <c r="D153" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E153" s="32" t="s">
+      <c r="E153" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F153" s="33"/>
-      <c r="G153" s="33"/>
-      <c r="H153" s="34"/>
+      <c r="F153" s="32"/>
+      <c r="G153" s="32"/>
+      <c r="H153" s="33"/>
       <c r="I153" s="2" t="s">
         <v>5</v>
       </c>
@@ -4778,7 +4766,7 @@
     </row>
     <row r="157" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="B157" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>75</v>
@@ -4790,26 +4778,22 @@
         <v>148</v>
       </c>
       <c r="D158" t="s">
+        <v>150</v>
+      </c>
+      <c r="L158" s="27"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
         <v>149</v>
       </c>
-      <c r="L158" s="27"/>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B159" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C159" s="31"/>
-      <c r="D159" s="31" t="s">
-        <v>150</v>
+      <c r="D159" t="s">
+        <v>151</v>
       </c>
       <c r="L159" s="27"/>
     </row>
-    <row r="160" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>151</v>
-      </c>
-      <c r="D160" s="24" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="L160" s="27"/>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Breathing system + Footsteps on every levels + Peristant audio""
This reverts commit e1790fd01841a3a68915eed2084d773b304ec2d4.
</commit_message>
<xml_diff>
--- a/BehindClosedDoors_SoundAssetList.xlsx
+++ b/BehindClosedDoors_SoundAssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\ISE 2\BehindClosedDoors_Git\BehindClosedDoors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F38AF-7F70-41D3-9E18-4799CA63794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6D877-9A83-4B0D-A529-4BD47BED6044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16080" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="164">
   <si>
     <t>Bible Asset List Library</t>
   </si>
@@ -584,9 +584,6 @@
     <t>RTPC_PLYR_WetFeet</t>
   </si>
   <si>
-    <t>RTPC_PLYR_FS</t>
-  </si>
-  <si>
     <t>Adapt wet level after walking over wet/water surface</t>
   </si>
   <si>
@@ -624,13 +621,20 @@
   </si>
   <si>
     <t>PLYR_FS_Carpet_Sneak</t>
+  </si>
+  <si>
+    <t>Increase over progression (After each Clue) + climax on Tunnel
+Impact on Amb + RTPC_PLYR_SelfConscious minimum &amp; Recovery time</t>
+  </si>
+  <si>
+    <t>RTPC_PLYR_FS_State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +660,13 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -980,6 +991,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1311,8 +1323,8 @@
   </sheetPr>
   <dimension ref="A1:R173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,12 +1352,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1359,14 +1371,14 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="33"/>
+      <c r="Q1" s="34"/>
       <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1400,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1520,7 +1532,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1620,7 +1632,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1959,7 +1971,7 @@
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
         <v>66</v>
@@ -2850,7 +2862,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
@@ -2858,7 +2870,7 @@
       <c r="Q66" s="7"/>
       <c r="R66" s="11"/>
     </row>
-    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="11" t="s">
         <v>106</v>
@@ -2876,7 +2888,7 @@
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
       <c r="M67" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -2884,7 +2896,7 @@
       <c r="Q67" s="7"/>
       <c r="R67" s="11"/>
     </row>
-    <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="7" t="s">
         <v>107</v>
@@ -2902,7 +2914,7 @@
       <c r="K68" s="7"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -2910,7 +2922,7 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="11"/>
     </row>
-    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2924,7 +2936,7 @@
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -2932,7 +2944,7 @@
       <c r="Q69" s="7"/>
       <c r="R69" s="11"/>
     </row>
-    <row r="70" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2946,7 +2958,7 @@
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
@@ -2954,7 +2966,7 @@
       <c r="Q70" s="7"/>
       <c r="R70" s="11"/>
     </row>
-    <row r="71" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>114</v>
       </c>
@@ -2974,7 +2986,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
@@ -2982,7 +2994,7 @@
       <c r="Q71" s="7"/>
       <c r="R71" s="11"/>
     </row>
-    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
         <v>112</v>
@@ -3000,7 +3012,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
@@ -3008,7 +3020,7 @@
       <c r="Q72" s="7"/>
       <c r="R72" s="11"/>
     </row>
-    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="7" t="s">
         <v>113</v>
@@ -3026,7 +3038,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3034,7 +3046,7 @@
       <c r="Q73" s="7"/>
       <c r="R73" s="11"/>
     </row>
-    <row r="74" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="7" t="s">
         <v>118</v>
@@ -3052,7 +3064,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3060,7 +3072,7 @@
       <c r="Q74" s="7"/>
       <c r="R74" s="11"/>
     </row>
-    <row r="75" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
         <v>119</v>
@@ -3078,7 +3090,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
@@ -3104,7 +3116,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3112,7 +3124,7 @@
       <c r="Q76" s="7"/>
       <c r="R76" s="11"/>
     </row>
-    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="7" t="s">
         <v>124</v>
@@ -3130,7 +3142,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
@@ -3138,7 +3150,7 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="11"/>
     </row>
-    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="7" t="s">
         <v>126</v>
@@ -3156,7 +3168,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
@@ -3164,14 +3176,14 @@
       <c r="Q78" s="7"/>
       <c r="R78" s="11"/>
     </row>
-    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="7"/>
@@ -3182,7 +3194,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -3190,7 +3202,7 @@
       <c r="Q79" s="7"/>
       <c r="R79" s="11"/>
     </row>
-    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="30" t="s">
         <v>128</v>
@@ -3208,7 +3220,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
@@ -3216,7 +3228,7 @@
       <c r="Q80" s="7"/>
       <c r="R80" s="11"/>
     </row>
-    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="7" t="s">
         <v>130</v>
@@ -3234,7 +3246,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
@@ -3284,7 +3296,7 @@
       <c r="Q83" s="7"/>
       <c r="R83" s="11"/>
     </row>
-    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>133</v>
       </c>
@@ -3306,7 +3318,7 @@
       <c r="K84" s="7"/>
       <c r="L84" s="7"/>
       <c r="M84" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -3404,7 +3416,7 @@
       <c r="Q88" s="7"/>
       <c r="R88" s="11"/>
     </row>
-    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="7" t="s">
         <v>145</v>
@@ -3622,7 +3634,7 @@
       <c r="Q98" s="7"/>
       <c r="R98" s="11"/>
     </row>
-    <row r="99" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="7" t="s">
         <v>96</v>
@@ -3903,11 +3915,11 @@
     <row r="111" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -4591,12 +4603,12 @@
       <c r="D144" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E144" s="31" t="s">
+      <c r="E144" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F144" s="32"/>
-      <c r="G144" s="32"/>
-      <c r="H144" s="33"/>
+      <c r="F144" s="33"/>
+      <c r="G144" s="33"/>
+      <c r="H144" s="34"/>
       <c r="I144" s="2" t="s">
         <v>5</v>
       </c>
@@ -4708,12 +4720,12 @@
       <c r="D153" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E153" s="31" t="s">
+      <c r="E153" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F153" s="32"/>
-      <c r="G153" s="32"/>
-      <c r="H153" s="33"/>
+      <c r="F153" s="33"/>
+      <c r="G153" s="33"/>
+      <c r="H153" s="34"/>
       <c r="I153" s="2" t="s">
         <v>5</v>
       </c>
@@ -4766,7 +4778,7 @@
     </row>
     <row r="157" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="B157" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>75</v>
@@ -4778,22 +4790,26 @@
         <v>148</v>
       </c>
       <c r="D158" t="s">
+        <v>149</v>
+      </c>
+      <c r="L158" s="27"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B159" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C159" s="31"/>
+      <c r="D159" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="L158" s="27"/>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>149</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="L159" s="27"/>
+    </row>
+    <row r="160" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
         <v>151</v>
       </c>
-      <c r="L159" s="27"/>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>152</v>
+      <c r="D160" s="24" t="s">
+        <v>162</v>
       </c>
       <c r="L160" s="27"/>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Breathing system + Footsteps on every levels + Peristant audio"""
This reverts commit 01c076cf7f62db6179c9fc901ad945763a3b84ed.
</commit_message>
<xml_diff>
--- a/BehindClosedDoors_SoundAssetList.xlsx
+++ b/BehindClosedDoors_SoundAssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\ISE 2\BehindClosedDoors_Git\BehindClosedDoors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6D877-9A83-4B0D-A529-4BD47BED6044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F38AF-7F70-41D3-9E18-4799CA63794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16080" xr2:uid="{D6966E3A-088F-4B41-946F-FE7DBD20A81C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="163">
   <si>
     <t>Bible Asset List Library</t>
   </si>
@@ -584,6 +584,9 @@
     <t>RTPC_PLYR_WetFeet</t>
   </si>
   <si>
+    <t>RTPC_PLYR_FS</t>
+  </si>
+  <si>
     <t>Adapt wet level after walking over wet/water surface</t>
   </si>
   <si>
@@ -621,20 +624,13 @@
   </si>
   <si>
     <t>PLYR_FS_Carpet_Sneak</t>
-  </si>
-  <si>
-    <t>Increase over progression (After each Clue) + climax on Tunnel
-Impact on Amb + RTPC_PLYR_SelfConscious minimum &amp; Recovery time</t>
-  </si>
-  <si>
-    <t>RTPC_PLYR_FS_State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,13 +656,6 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -901,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -991,7 +980,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1323,8 +1311,8 @@
   </sheetPr>
   <dimension ref="A1:R173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,12 +1340,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1371,14 +1359,14 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="34"/>
+      <c r="Q1" s="33"/>
       <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1412,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1532,7 +1520,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1632,7 +1620,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1971,7 +1959,7 @@
       </c>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7" t="s">
         <v>66</v>
@@ -2862,7 +2850,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
@@ -2870,7 +2858,7 @@
       <c r="Q66" s="7"/>
       <c r="R66" s="11"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="11" t="s">
         <v>106</v>
@@ -2888,7 +2876,7 @@
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
       <c r="M67" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
@@ -2896,7 +2884,7 @@
       <c r="Q67" s="7"/>
       <c r="R67" s="11"/>
     </row>
-    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="7" t="s">
         <v>107</v>
@@ -2914,7 +2902,7 @@
       <c r="K68" s="7"/>
       <c r="L68" s="7"/>
       <c r="M68" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -2922,7 +2910,7 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="11"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2936,7 +2924,7 @@
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
       <c r="M69" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
@@ -2944,7 +2932,7 @@
       <c r="Q69" s="7"/>
       <c r="R69" s="11"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2958,7 +2946,7 @@
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
@@ -2966,7 +2954,7 @@
       <c r="Q70" s="7"/>
       <c r="R70" s="11"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>114</v>
       </c>
@@ -2986,7 +2974,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
@@ -2994,7 +2982,7 @@
       <c r="Q71" s="7"/>
       <c r="R71" s="11"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
         <v>112</v>
@@ -3012,7 +3000,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
@@ -3020,7 +3008,7 @@
       <c r="Q72" s="7"/>
       <c r="R72" s="11"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="7" t="s">
         <v>113</v>
@@ -3038,7 +3026,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
@@ -3046,7 +3034,7 @@
       <c r="Q73" s="7"/>
       <c r="R73" s="11"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="7" t="s">
         <v>118</v>
@@ -3064,7 +3052,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -3072,7 +3060,7 @@
       <c r="Q74" s="7"/>
       <c r="R74" s="11"/>
     </row>
-    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
         <v>119</v>
@@ -3090,7 +3078,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
@@ -3116,7 +3104,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
@@ -3124,7 +3112,7 @@
       <c r="Q76" s="7"/>
       <c r="R76" s="11"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="7" t="s">
         <v>124</v>
@@ -3142,7 +3130,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
@@ -3150,7 +3138,7 @@
       <c r="Q77" s="7"/>
       <c r="R77" s="11"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="7" t="s">
         <v>126</v>
@@ -3168,7 +3156,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
@@ -3176,14 +3164,14 @@
       <c r="Q78" s="7"/>
       <c r="R78" s="11"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="7"/>
@@ -3194,7 +3182,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
@@ -3202,7 +3190,7 @@
       <c r="Q79" s="7"/>
       <c r="R79" s="11"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="30" t="s">
         <v>128</v>
@@ -3220,7 +3208,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
       <c r="M80" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
@@ -3228,7 +3216,7 @@
       <c r="Q80" s="7"/>
       <c r="R80" s="11"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="7" t="s">
         <v>130</v>
@@ -3246,7 +3234,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
       <c r="M81" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
@@ -3296,7 +3284,7 @@
       <c r="Q83" s="7"/>
       <c r="R83" s="11"/>
     </row>
-    <row r="84" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>133</v>
       </c>
@@ -3318,7 +3306,7 @@
       <c r="K84" s="7"/>
       <c r="L84" s="7"/>
       <c r="M84" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
@@ -3416,7 +3404,7 @@
       <c r="Q88" s="7"/>
       <c r="R88" s="11"/>
     </row>
-    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="7" t="s">
         <v>145</v>
@@ -3634,7 +3622,7 @@
       <c r="Q98" s="7"/>
       <c r="R98" s="11"/>
     </row>
-    <row r="99" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="7" t="s">
         <v>96</v>
@@ -3915,11 +3903,11 @@
     <row r="111" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -4603,12 +4591,12 @@
       <c r="D144" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E144" s="32" t="s">
+      <c r="E144" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F144" s="33"/>
-      <c r="G144" s="33"/>
-      <c r="H144" s="34"/>
+      <c r="F144" s="32"/>
+      <c r="G144" s="32"/>
+      <c r="H144" s="33"/>
       <c r="I144" s="2" t="s">
         <v>5</v>
       </c>
@@ -4720,12 +4708,12 @@
       <c r="D153" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E153" s="32" t="s">
+      <c r="E153" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F153" s="33"/>
-      <c r="G153" s="33"/>
-      <c r="H153" s="34"/>
+      <c r="F153" s="32"/>
+      <c r="G153" s="32"/>
+      <c r="H153" s="33"/>
       <c r="I153" s="2" t="s">
         <v>5</v>
       </c>
@@ -4778,7 +4766,7 @@
     </row>
     <row r="157" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="B157" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D157" s="24" t="s">
         <v>75</v>
@@ -4790,26 +4778,22 @@
         <v>148</v>
       </c>
       <c r="D158" t="s">
+        <v>150</v>
+      </c>
+      <c r="L158" s="27"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
         <v>149</v>
       </c>
-      <c r="L158" s="27"/>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B159" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C159" s="31"/>
-      <c r="D159" s="31" t="s">
-        <v>150</v>
+      <c r="D159" t="s">
+        <v>151</v>
       </c>
       <c r="L159" s="27"/>
     </row>
-    <row r="160" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>151</v>
-      </c>
-      <c r="D160" s="24" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="L160" s="27"/>
     </row>

</xml_diff>